<commit_message>
grouped test files, updated results
</commit_message>
<xml_diff>
--- a/Test sentences CUT and NORMALIZED/Test distribution.xlsx
+++ b/Test sentences CUT and NORMALIZED/Test distribution.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760" activeTab="1"/>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Setup" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="65">
   <si>
     <t>Block 1</t>
   </si>
@@ -99,6 +101,126 @@
   </si>
   <si>
     <t>mening05_02</t>
+  </si>
+  <si>
+    <t>Understood sentence</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>mening02-02</t>
+  </si>
+  <si>
+    <t>mening02-04</t>
+  </si>
+  <si>
+    <t>… tunnelbana</t>
+  </si>
+  <si>
+    <t>… buskarna</t>
+  </si>
+  <si>
+    <t>Snabbt till marken</t>
+  </si>
+  <si>
+    <t>Hur var det i skolan igår?</t>
+  </si>
+  <si>
+    <t>Ursäkta har du biljetten?</t>
+  </si>
+  <si>
+    <t>… tillkalla polisen</t>
+  </si>
+  <si>
+    <t>handduken låg på golvet</t>
+  </si>
+  <si>
+    <t>tjuren jagade mannen</t>
+  </si>
+  <si>
+    <t>grannen knackade på dörren</t>
+  </si>
+  <si>
+    <t>brevlådan är nyligen tömd</t>
+  </si>
+  <si>
+    <t>mamma skakade på huvudet</t>
+  </si>
+  <si>
+    <t>den gamla damen drog barnvagnen</t>
+  </si>
+  <si>
+    <t>dom nya skorna var trånga</t>
+  </si>
+  <si>
+    <t>kappan hänger i garderoben</t>
+  </si>
+  <si>
+    <t>solen lyste genom molnen</t>
+  </si>
+  <si>
+    <t>han bar på ett paraply</t>
+  </si>
+  <si>
+    <t>de går snabbt genom parken</t>
+  </si>
+  <si>
+    <t>någon gömmer sig i buskarna</t>
+  </si>
+  <si>
+    <t>kyparen tände ljusen</t>
+  </si>
+  <si>
+    <t>kvinnan halkade på isen</t>
+  </si>
+  <si>
+    <t>flickan började skolan igår</t>
+  </si>
+  <si>
+    <t>de köpte några biljetter</t>
+  </si>
+  <si>
+    <t>sköterskan hjälpte barnet</t>
+  </si>
+  <si>
+    <t>doktorn bar en svart väska</t>
+  </si>
+  <si>
+    <t>comprehensibility</t>
+  </si>
+  <si>
+    <t>pleasantness</t>
+  </si>
+  <si>
+    <t>deviation</t>
+  </si>
+  <si>
+    <t>Deviation</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Swedish</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>26-30</t>
+  </si>
+  <si>
+    <t>Native</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>21-25</t>
   </si>
 </sst>
 </file>
@@ -427,8 +549,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,4 +916,666 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BX6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="23" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:76" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BI1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" t="s">
+        <v>56</v>
+      </c>
+      <c r="S2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" t="s">
+        <v>56</v>
+      </c>
+      <c r="W2" t="s">
+        <v>53</v>
+      </c>
+      <c r="X2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>56</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>56</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>56</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>56</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>56</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>56</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3">
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3">
+        <v>4</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>3</v>
+      </c>
+      <c r="U3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V3">
+        <v>4</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>3</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3">
+        <v>5</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>4</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD3">
+        <v>5</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>2</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH3">
+        <v>4</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3">
+        <v>2</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL3">
+        <v>4</v>
+      </c>
+      <c r="AM3">
+        <v>1</v>
+      </c>
+      <c r="AN3">
+        <v>2</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AP3">
+        <v>5</v>
+      </c>
+      <c r="AQ3">
+        <v>1</v>
+      </c>
+      <c r="AR3">
+        <v>2</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AT3">
+        <v>4</v>
+      </c>
+      <c r="AU3">
+        <v>2</v>
+      </c>
+      <c r="AV3">
+        <v>2</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AX3">
+        <v>4</v>
+      </c>
+      <c r="AY3">
+        <v>2</v>
+      </c>
+      <c r="AZ3">
+        <v>2</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>26</v>
+      </c>
+      <c r="BB3">
+        <v>3</v>
+      </c>
+      <c r="BC3">
+        <v>1</v>
+      </c>
+      <c r="BD3">
+        <v>2</v>
+      </c>
+      <c r="BE3" t="s">
+        <v>34</v>
+      </c>
+      <c r="BF3">
+        <v>4</v>
+      </c>
+      <c r="BG3">
+        <v>2</v>
+      </c>
+      <c r="BH3">
+        <v>2</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>32</v>
+      </c>
+      <c r="BJ3">
+        <v>2</v>
+      </c>
+      <c r="BK3">
+        <v>3</v>
+      </c>
+      <c r="BL3">
+        <v>2</v>
+      </c>
+      <c r="BM3" t="s">
+        <v>26</v>
+      </c>
+      <c r="BN3">
+        <v>5</v>
+      </c>
+      <c r="BO3">
+        <v>1</v>
+      </c>
+      <c r="BP3">
+        <v>2</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>33</v>
+      </c>
+      <c r="BR3">
+        <v>3</v>
+      </c>
+      <c r="BS3">
+        <v>3</v>
+      </c>
+      <c r="BT3">
+        <v>2</v>
+      </c>
+      <c r="BU3" t="s">
+        <v>29</v>
+      </c>
+      <c r="BV3">
+        <v>3</v>
+      </c>
+      <c r="BW3">
+        <v>2</v>
+      </c>
+      <c r="BX3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>